<commit_message>
Minor revision on the dashboard sheet
</commit_message>
<xml_diff>
--- a/Data Analysis/Alumni Tracer CS JHS/Excel/Alumni Tracer CS JHS.xlsx
+++ b/Data Analysis/Alumni Tracer CS JHS/Excel/Alumni Tracer CS JHS.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d9fa0445d99ba1a7/Documents/__Learning/Portfolio/Data Analysis/Alumni Tracer CS JHS/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{147E5ACC-3127-4FED-8D94-7C3D7E93F375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{147E5ACC-3127-4FED-8D94-7C3D7E93F375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39408156-D462-4BF9-B74F-EFE1AAEFE361}"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="1260" windowWidth="24345" windowHeight="18630" activeTab="5"/>
+    <workbookView xWindow="24435" yWindow="1830" windowWidth="26295" windowHeight="18630" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -30,17 +30,17 @@
     <definedName name="Slicer_Lanjut_ke_Sekolah_Menengah_...">#N/A</definedName>
     <definedName name="Slicer_Lulus_dari_SPENSANA__...">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="539" r:id="rId7"/>
-    <pivotCache cacheId="542" r:id="rId8"/>
-    <pivotCache cacheId="545" r:id="rId9"/>
-    <pivotCache cacheId="548" r:id="rId10"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="2" r:id="rId9"/>
+    <pivotCache cacheId="3" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{876F7934-8845-4945-9796-88D515C7AA90}">
       <x14:pivotCaches>
-        <pivotCache cacheId="514" r:id="rId11"/>
+        <pivotCache cacheId="4" r:id="rId11"/>
       </x14:pivotCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -61,13 +61,22 @@
         </x15:modelTables>
       </x15:dataModel>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="ThisWorkbookDataModel" description="Data Model" type="5" refreshedVersion="7" minRefreshableVersion="5" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="ThisWorkbookDataModel" description="Data Model" type="5" refreshedVersion="7" minRefreshableVersion="5" background="1">
     <dbPr connection="Data Model Connection" command="Model" commandType="1"/>
     <olapPr sendLocale="1" rowDrillCount="1000"/>
     <extLst>
@@ -76,7 +85,7 @@
       </ext>
     </extLst>
   </connection>
-  <connection id="2" name="WorksheetConnection_cleaned!$A$1:$F$122" type="102" refreshedVersion="7" minRefreshableVersion="5">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="WorksheetConnection_cleaned!$A$1:$F$122" type="102" refreshedVersion="7" minRefreshableVersion="5">
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
@@ -1347,7 +1356,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1895,17 +1904,17 @@
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2098,6 +2107,34 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -2131,6 +2168,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-7D25-4DB1-8B3B-53949437D33E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2146,6 +2188,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-7D25-4DB1-8B3B-53949437D33E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -12031,8 +12078,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="6" name="Jenis Kelamin">
@@ -12055,7 +12102,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -12223,8 +12270,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>153866</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="10" name="Lulus dari SPENSANA  ...">
@@ -12247,7 +12294,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -12301,8 +12348,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="11" name="Lanjut ke Sekolah Menengah ...">
@@ -12325,7 +12372,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -12376,8 +12423,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>122117</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -12392,8 +12439,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12011025" y="1657350"/>
-          <a:ext cx="1695450" cy="2019300"/>
+          <a:off x="12103100" y="1986573"/>
+          <a:ext cx="1691542" cy="2409582"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12459,7 +12506,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>76%</a:t>
+            <a:t>63%</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100">
@@ -12644,14 +12691,14 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>187568</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>109903</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -12666,8 +12713,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12011025" y="3714750"/>
-          <a:ext cx="1685925" cy="2019300"/>
+          <a:off x="12103100" y="4461606"/>
+          <a:ext cx="1682017" cy="2266951"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12865,8 +12912,8 @@
       <xdr:row>47</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="14" name="Fakultas">
@@ -12889,7 +12936,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -12934,7 +12981,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Zelvy Fauzan" refreshedDate="46016.669412268522" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Zelvy Fauzan" refreshedDate="46016.669412268522" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF1B020000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="2">
     <cacheField name="[Measures].[Count of Lanjut ke Sekolah Menengah ...]" caption="Count of Lanjut ke Sekolah Menengah ..." numFmtId="0" hierarchy="9" level="32767"/>
@@ -13011,7 +13058,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Zelvy Fauzan" refreshedDate="46016.669412731484" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Zelvy Fauzan" refreshedDate="46016.669412731484" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF1E020000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
     <cacheField name="[Range].[Jurusan …].[Jurusan …]" caption="Jurusan …" numFmtId="0" hierarchy="4" level="1">
@@ -13120,7 +13167,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Zelvy Fauzan" refreshedDate="46016.669413194446" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Zelvy Fauzan" refreshedDate="46016.669413194446" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF21020000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
     <cacheField name="[Range].[Fakultas].[Fakultas]" caption="Fakultas" numFmtId="0" hierarchy="5" level="1">
@@ -13214,7 +13261,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Zelvy Fauzan" refreshedDate="46016.669413657408" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Zelvy Fauzan" refreshedDate="46016.669413657408" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF24020000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="4">
     <cacheField name="[Range].[Lulus dari SPENSANA  ...].[Lulus dari SPENSANA  ...]" caption="Lulus dari SPENSANA  ..." numFmtId="0" hierarchy="2" level="1">
@@ -13331,7 +13378,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Zelvy Fauzan" refreshedDate="46016.669158680554" backgroundQuery="1" createdVersion="3" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Zelvy Fauzan" refreshedDate="46016.669158680554" backgroundQuery="1" createdVersion="3" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF02020000}">
   <cacheSource type="external" connectionId="1">
     <extLst>
       <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{F057638F-6D5F-4e77-A914-E7F072B9BCA8}">
@@ -13388,7 +13435,333 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable9" cacheId="548" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000001000000}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A16:B43" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="26">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="27">
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Jurusan …" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotHierarchies count="12">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
+    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
+    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="4"/>
+  </rowHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_cleaned!$A$1:$F$122">
+        <x15:activeTabTopLevelEntity name="[Range]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A1:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="2">
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Lanjut ke Sekolah Menengah ..." fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="6">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotHierarchies count="12">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
+    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
+    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="3"/>
+  </rowHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_cleaned!$A$1:$F$122">
+        <x15:activeTabTopLevelEntity name="[Range]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000003000000}" name="PivotTable9" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A65:B96" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -13586,8 +13959,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable8" cacheId="545" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000002000000}" name="PivotTable8" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A47:B59" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -13718,308 +14091,6 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="542" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A16:B43" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="26">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="27">
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Jurusan …" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotHierarchies count="12">
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
-    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
-    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-  </pivotHierarchies>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <rowHierarchiesUsage count="1">
-    <rowHierarchyUsage hierarchyUsage="4"/>
-  </rowHierarchiesUsage>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
-      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_cleaned!$A$1:$F$122">
-        <x15:activeTabTopLevelEntity name="[Range]"/>
-      </x15:pivotTableUISettings>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="539" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A1:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="2">
-        <item x="0"/>
-        <item x="1"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Lanjut ke Sekolah Menengah ..." fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="4">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotHierarchies count="12">
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
-    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
-    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-  </pivotHierarchies>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <rowHierarchiesUsage count="1">
-    <rowHierarchyUsage hierarchyUsage="3"/>
-  </rowHierarchiesUsage>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
-      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_cleaned!$A$1:$F$122">
-        <x15:activeTabTopLevelEntity name="[Range]"/>
-      </x15:pivotTableUISettings>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
 <rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <global>
@@ -14083,7 +14154,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Jenis_Kelamin" sourceName="[Range].[Jenis Kelamin]">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Jenis_Kelamin" xr10:uid="{00000000-0013-0000-FFFF-FFFF01000000}" sourceName="[Range].[Jenis Kelamin]">
   <pivotTables>
     <pivotTable tabId="5" name="PivotTable1"/>
     <pivotTable tabId="5" name="PivotTable5"/>
@@ -14112,7 +14183,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Lulus_dari_SPENSANA__..." sourceName="[Range].[Lulus dari SPENSANA  ...]">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Lulus_dari_SPENSANA__..." xr10:uid="{00000000-0013-0000-FFFF-FFFF02000000}" sourceName="[Range].[Lulus dari SPENSANA  ...]">
   <pivotTables>
     <pivotTable tabId="5" name="PivotTable1"/>
     <pivotTable tabId="5" name="PivotTable5"/>
@@ -14142,7 +14213,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Lanjut_ke_Sekolah_Menengah_..." sourceName="[Range].[Lanjut ke Sekolah Menengah ...]">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Lanjut_ke_Sekolah_Menengah_..." xr10:uid="{00000000-0013-0000-FFFF-FFFF03000000}" sourceName="[Range].[Lanjut ke Sekolah Menengah ...]">
   <pivotTables>
     <pivotTable tabId="5" name="PivotTable1"/>
     <pivotTable tabId="5" name="PivotTable5"/>
@@ -14171,7 +14242,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache4.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Fakultas" sourceName="[Range].[Fakultas]">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Fakultas" xr10:uid="{00000000-0013-0000-FFFF-FFFF04000000}" sourceName="[Range].[Fakultas]">
   <pivotTables>
     <pivotTable tabId="5" name="PivotTable1"/>
     <pivotTable tabId="5" name="PivotTable5"/>
@@ -14209,11 +14280,11 @@
 </file>
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <slicer name="Jenis Kelamin" cache="Slicer_Jenis_Kelamin" caption="Jenis Kelamin" level="1" rowHeight="257175"/>
-  <slicer name="Lulus dari SPENSANA  ..." cache="Slicer_Lulus_dari_SPENSANA__..." caption="Lulus dari SPENSANA  ..." level="1" rowHeight="257175"/>
-  <slicer name="Lanjut ke Sekolah Menengah ..." cache="Slicer_Lanjut_ke_Sekolah_Menengah_..." caption="Lanjut ke Sekolah Menengah ..." level="1" rowHeight="257175"/>
-  <slicer name="Fakultas" cache="Slicer_Fakultas" caption="Fakultas" level="1" rowHeight="257175"/>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Jenis Kelamin" xr10:uid="{00000000-0014-0000-FFFF-FFFF01000000}" cache="Slicer_Jenis_Kelamin" caption="Jenis Kelamin" level="1" rowHeight="257175"/>
+  <slicer name="Lulus dari SPENSANA  ..." xr10:uid="{00000000-0014-0000-FFFF-FFFF02000000}" cache="Slicer_Lulus_dari_SPENSANA__..." caption="Lulus dari SPENSANA  ..." level="1" rowHeight="257175"/>
+  <slicer name="Lanjut ke Sekolah Menengah ..." xr10:uid="{00000000-0014-0000-FFFF-FFFF03000000}" cache="Slicer_Lanjut_ke_Sekolah_Menengah_..." caption="Lanjut ke Sekolah Menengah ..." level="1" rowHeight="257175"/>
+  <slicer name="Fakultas" xr10:uid="{00000000-0014-0000-FFFF-FFFF04000000}" cache="Slicer_Fakultas" caption="Fakultas" level="1" rowHeight="257175"/>
 </slicers>
 </file>
 
@@ -14513,7 +14584,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16969,7 +17040,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H122"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -19700,14 +19771,14 @@
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="aob98pq8XMssePbfr51cIx5XXmORVg2EKiPBf0S8dadi9874Zwgs9uZt46pjASRZR3UJKipkvgEdKhGdh1bUSA==" saltValue="lpQF0sSZWc2uiSnnAdba/w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <autoFilter ref="A1:F122"/>
+  <autoFilter ref="A1:F122" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22706,7 +22777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25161,13 +25232,13 @@
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="KJ+8RRRS2nVHZZn99Qibl2tS3fcBRMmzMhcyPf+fEHLaoGpgd6g4g/8XiAW8uDSHubkKixkQDKs8FzNqFKRCWw==" saltValue="FA/d0PGjMw2xlAuoove+9w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <autoFilter ref="A1:F122"/>
+  <autoFilter ref="A1:F122" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25798,10 +25869,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
@@ -25815,138 +25886,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
     </row>
     <row r="6" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
     </row>
     <row r="7" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -25954,29 +26025,29 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="14" t="s">
         <v>378</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15" t="s">
+      <c r="G7" s="13"/>
+      <c r="H7" s="13" t="s">
         <v>383</v>
       </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="16" t="s">
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15" t="s">
+      <c r="L7" s="13"/>
+      <c r="M7" s="13" t="s">
         <v>380</v>
       </c>
       <c r="N7" s="8"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
     </row>
     <row r="8" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
@@ -25984,29 +26055,29 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="14" t="s">
         <v>376</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15" t="s">
+      <c r="G8" s="13"/>
+      <c r="H8" s="13" t="s">
         <v>377</v>
       </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="16" t="s">
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="14" t="s">
         <v>381</v>
       </c>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15" t="s">
+      <c r="L8" s="13"/>
+      <c r="M8" s="13" t="s">
         <v>382</v>
       </c>
       <c r="N8" s="8"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
     </row>
     <row r="9" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
@@ -26014,27 +26085,27 @@
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
       <c r="N9" s="8"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="15"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>

</xml_diff>